<commit_message>
Todo en la misma hoja de Excel
</commit_message>
<xml_diff>
--- a/test/Happy.xlsx
+++ b/test/Happy.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Evento_1</t>
   </si>
@@ -65,10 +65,46 @@
     <t>categoría_1</t>
   </si>
   <si>
-    <t>categoría_4</t>
-  </si>
-  <si>
-    <t>categoría_5</t>
+    <t>Organización_1</t>
+  </si>
+  <si>
+    <t>Organización_3</t>
+  </si>
+  <si>
+    <t>Organización_4</t>
+  </si>
+  <si>
+    <t>Nombre_1 Apellido_1 Segundo_1 | Qa</t>
+  </si>
+  <si>
+    <t>Nombre_3 Apellido_3 Segundo_3 | Segundo_</t>
+  </si>
+  <si>
+    <t>Nombre_4 Apellido_4 Segundo_4 | Segun</t>
+  </si>
+  <si>
+    <t>Demo del acuerdo numero_1</t>
+  </si>
+  <si>
+    <t>Demo del acuerdo numero_2</t>
+  </si>
+  <si>
+    <t>Demo del acuerdo numero_3</t>
+  </si>
+  <si>
+    <t>sigla_1</t>
+  </si>
+  <si>
+    <t>categoría_2</t>
+  </si>
+  <si>
+    <t>sigla_2</t>
+  </si>
+  <si>
+    <t>categoría_3</t>
+  </si>
+  <si>
+    <t>sigla_3</t>
   </si>
 </sst>
 </file>
@@ -395,19 +431,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.21875" customWidth="1"/>
     <col min="7" max="7" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="10" max="10" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -429,11 +468,30 @@
       <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="str">
+        <f>M1</f>
+        <v>categoría_1</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="N1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -455,11 +513,30 @@
       <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H2" t="str">
+        <f t="shared" ref="H2:H3" si="0">M2</f>
+        <v>categoría_2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -481,12 +558,58 @@
       <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H3" t="str">
+        <f t="shared" si="0"/>
+        <v>categoría_3</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Termina carga excel completa
</commit_message>
<xml_diff>
--- a/test/Happy.xlsx
+++ b/test/Happy.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="66">
   <si>
     <t>Evento_1</t>
   </si>
@@ -74,15 +75,6 @@
     <t>Organización_4</t>
   </si>
   <si>
-    <t>Nombre_1 Apellido_1 Segundo_1 | Qa</t>
-  </si>
-  <si>
-    <t>Nombre_3 Apellido_3 Segundo_3 | Segundo_</t>
-  </si>
-  <si>
-    <t>Nombre_4 Apellido_4 Segundo_4 | Segun</t>
-  </si>
-  <si>
     <t>Demo del acuerdo numero_1</t>
   </si>
   <si>
@@ -95,9 +87,6 @@
     <t>sigla_1</t>
   </si>
   <si>
-    <t>categoría_2</t>
-  </si>
-  <si>
     <t>sigla_2</t>
   </si>
   <si>
@@ -105,6 +94,135 @@
   </si>
   <si>
     <t>sigla_3</t>
+  </si>
+  <si>
+    <t>Evento_4</t>
+  </si>
+  <si>
+    <t>Datos de prueba del evento_4</t>
+  </si>
+  <si>
+    <t>categoría_4</t>
+  </si>
+  <si>
+    <t>sigla_4</t>
+  </si>
+  <si>
+    <t>Org_1</t>
+  </si>
+  <si>
+    <t>Organización_2</t>
+  </si>
+  <si>
+    <t>Org_2</t>
+  </si>
+  <si>
+    <t>Org_3</t>
+  </si>
+  <si>
+    <t>Org_4</t>
+  </si>
+  <si>
+    <t>categoría_5</t>
+  </si>
+  <si>
+    <t>Cargo_1</t>
+  </si>
+  <si>
+    <t>Cargo_2</t>
+  </si>
+  <si>
+    <t>Cargo_3</t>
+  </si>
+  <si>
+    <t>Cargo_4</t>
+  </si>
+  <si>
+    <t>Nombre_1</t>
+  </si>
+  <si>
+    <t>Nombre_3</t>
+  </si>
+  <si>
+    <t>Nombre_4</t>
+  </si>
+  <si>
+    <t>Nombre_5</t>
+  </si>
+  <si>
+    <t>Nombre_2</t>
+  </si>
+  <si>
+    <t>Ap_1</t>
+  </si>
+  <si>
+    <t>Ap_2</t>
+  </si>
+  <si>
+    <t>Ap_3</t>
+  </si>
+  <si>
+    <t>Ap_4</t>
+  </si>
+  <si>
+    <t>Am_1</t>
+  </si>
+  <si>
+    <t>Am_2</t>
+  </si>
+  <si>
+    <t>Am_3</t>
+  </si>
+  <si>
+    <t>Am_4</t>
+  </si>
+  <si>
+    <t>Nombre_1 Ap_1 Am_1 | Cargo_1</t>
+  </si>
+  <si>
+    <t>Nombre_2 Ap_2 Am_2 | Cargo_2</t>
+  </si>
+  <si>
+    <t>Nombre_3 Ap_3 Am_3 | Cargo_3</t>
+  </si>
+  <si>
+    <t>Nombre_4 Ap_4 Am_4 | Cargo_4</t>
+  </si>
+  <si>
+    <t>Evento_5</t>
+  </si>
+  <si>
+    <t>Datos de prueba del evento_5</t>
+  </si>
+  <si>
+    <t>Demo del acuerdo numero_5</t>
+  </si>
+  <si>
+    <t>Demo del acuerdo numero_4</t>
+  </si>
+  <si>
+    <t>categoría_6</t>
+  </si>
+  <si>
+    <t>sigla_7</t>
+  </si>
+  <si>
+    <t>Organización_5</t>
+  </si>
+  <si>
+    <t>Org_5</t>
+  </si>
+  <si>
+    <t>Cargo_5</t>
+  </si>
+  <si>
+    <t>Ap_5</t>
+  </si>
+  <si>
+    <t>Am_5</t>
+  </si>
+  <si>
+    <t>Nombre_5 Ap_5 Am_5 | Cargo_5</t>
   </si>
 </sst>
 </file>
@@ -128,12 +246,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -148,14 +272,46 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -431,22 +587,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.21875" customWidth="1"/>
-    <col min="7" max="7" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" style="5"/>
+    <col min="9" max="9" width="13.6640625" style="5" customWidth="1"/>
     <col min="10" max="10" width="38.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="30.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -468,18 +627,20 @@
       <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="str">
+      <c r="H1" s="5" t="str">
         <f>M1</f>
         <v>categoría_1</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="I1" s="6" t="str">
+        <f>O1</f>
+        <v>Organización_1</v>
+      </c>
+      <c r="J1" s="3" t="str">
+        <f>CONCATENATE(R1," ",S1," ",T1," ","| ",Q1)</f>
+        <v>Nombre_1 Ap_1 Am_1 | Cargo_1</v>
+      </c>
+      <c r="K1" t="s">
         <v>16</v>
-      </c>
-      <c r="K1" t="s">
-        <v>19</v>
       </c>
       <c r="L1" t="s">
         <v>4</v>
@@ -488,10 +649,31 @@
         <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -513,30 +695,53 @@
       <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" t="str">
+      <c r="H2" s="5" t="str">
         <f t="shared" ref="H2:H3" si="0">M2</f>
-        <v>categoría_2</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
+        <v>categoría_3</v>
+      </c>
+      <c r="I2" s="6" t="str">
+        <f t="shared" ref="I2:I4" si="1">O2</f>
+        <v>Organización_2</v>
+      </c>
+      <c r="J2" s="3" t="str">
+        <f t="shared" ref="J2:J4" si="2">CONCATENATE(R2," ",S2," ",T2," ","| ",Q2)</f>
+        <v>Nombre_2 Ap_2 Am_2 | Cargo_2</v>
+      </c>
+      <c r="K2" t="s">
         <v>17</v>
-      </c>
-      <c r="K2" t="s">
-        <v>20</v>
       </c>
       <c r="L2" t="s">
         <v>5</v>
       </c>
       <c r="M2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="N2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="O2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="U2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -558,18 +763,20 @@
       <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="H3" t="str">
+      <c r="H3" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>categoría_3</v>
-      </c>
-      <c r="I3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" t="s">
+        <v>categoría_4</v>
+      </c>
+      <c r="I3" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Organización_3</v>
+      </c>
+      <c r="J3" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Nombre_3 Ap_3 Am_3 | Cargo_3</v>
+      </c>
+      <c r="K3" t="s">
         <v>18</v>
-      </c>
-      <c r="K3" t="s">
-        <v>21</v>
       </c>
       <c r="L3" t="s">
         <v>6</v>
@@ -578,36 +785,185 @@
         <v>25</v>
       </c>
       <c r="N3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="U3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4">
+        <v>17</v>
+      </c>
+      <c r="E4">
+        <v>11</v>
+      </c>
+      <c r="F4">
+        <v>40</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="5" t="str">
+        <f t="shared" ref="H4:H5" si="3">M4</f>
+        <v>categoría_5</v>
+      </c>
+      <c r="I4" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Organización_4</v>
+      </c>
+      <c r="J4" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Nombre_4 Ap_4 Am_4 | Cargo_4</v>
+      </c>
+      <c r="K4" t="s">
+        <v>57</v>
+      </c>
+      <c r="L4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P4" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="U4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5">
+        <v>18</v>
+      </c>
+      <c r="E5">
+        <v>12</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>categoría_6</v>
+      </c>
+      <c r="I5" s="6" t="str">
+        <f t="shared" ref="I5" si="4">O5</f>
+        <v>Organización_5</v>
+      </c>
+      <c r="J5" s="3" t="str">
+        <f t="shared" ref="J5" si="5">CONCATENATE(R5," ",S5," ",T5," ","| ",Q5)</f>
+        <v>Nombre_5 Ap_5 Am_5 | Cargo_5</v>
+      </c>
+      <c r="K5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M5" t="s">
+        <v>58</v>
+      </c>
+      <c r="N5" t="s">
+        <v>59</v>
+      </c>
+      <c r="O5" t="s">
+        <v>60</v>
+      </c>
+      <c r="P5" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="U5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="J6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="K10" s="4"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
@@ -615,4 +971,46 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="str">
+        <f>Hoja1!$J$1</f>
+        <v>Nombre_1 Ap_1 Am_1 | Cargo_1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="str">
+        <f>Hoja1!$J$1</f>
+        <v>Nombre_1 Ap_1 Am_1 | Cargo_1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="str">
+        <f>Hoja1!$J$1</f>
+        <v>Nombre_1 Ap_1 Am_1 | Cargo_1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="str">
+        <f>Hoja1!$J$1</f>
+        <v>Nombre_1 Ap_1 Am_1 | Cargo_1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>